<commit_message>
Con 11 es muy rígido. Probar otras secciones de rigidizadores
</commit_message>
<xml_diff>
--- a/MicroSat/Numeración.xlsx
+++ b/MicroSat/Numeración.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. EUE\Micro-Satellite Design &amp; Analysis\MicroSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DB620D-66B0-48FF-8517-B35BBE1E5A45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FDDE91-4D7E-4FE1-84A9-69730369719F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6F37F754-23FB-4F1B-8596-2383A88C50CE}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6F37F754-23FB-4F1B-8596-2383A88C50CE}"/>
   </bookViews>
   <sheets>
     <sheet name="It1 - 9 rig" sheetId="1" r:id="rId1"/>
     <sheet name="rect_Al7075_2mm_13x9.5_13x5" sheetId="2" r:id="rId2"/>
     <sheet name="rect_Al7075_3mm_13x13_13x9.5" sheetId="3" r:id="rId3"/>
     <sheet name="rect_Al7075_3mm_19x15_19x13" sheetId="4" r:id="rId4"/>
+    <sheet name="It1 - 11 rig" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>TIPO DE ELEMENTO</t>
   </si>
@@ -446,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -470,14 +471,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,6 +596,99 @@
         <a:xfrm>
           <a:off x="6785610" y="577215"/>
           <a:ext cx="9331428" cy="893334"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>591787</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>176599</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5466348-E1BB-42B1-8A5B-7AFDD9A56F7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2988945" y="0"/>
+          <a:ext cx="5346667" cy="4519999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>73148</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>50893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A347552B-E554-4936-AA43-40674BF02021}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8401050" y="57150"/>
+          <a:ext cx="9169523" cy="4337143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -888,7 +1000,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,7 +1072,7 @@
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
@@ -968,13 +1080,13 @@
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="12"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -982,7 +1094,7 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="10"/>
+      <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1021,7 +1133,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1191,7 +1303,7 @@
       <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1327,7 +1439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59C3F0D-D8B4-4BBB-96DC-630B235CEF9A}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -1352,7 +1464,7 @@
       <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1482,4 +1594,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6A597C-DEB9-47F1-8D76-6285F53F438F}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>